<commit_message>
moved formatting cells to the first row
</commit_message>
<xml_diff>
--- a/src/main/resources/org/jxls/demo/simple_export_template.xlsx
+++ b/src/main/resources/org/jxls/demo/simple_export_template.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Автор</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0">
@@ -40,7 +40,7 @@
           </rPr>
           <t xml:space="preserve">
 jx:area(lastCell="A2")
-jx:grid(lastCell="A2" headers="headers" data="data" areas=[A1:A1, A2:A2] formatCells="Integer:A3,Long:A3,Short:A3,Double:B3,Float:B3,BigDecimal:B3,Date:C3")</t>
+jx:grid(lastCell="A2" headers="headers" data="data" areas=[A1:A1, A2:A2] formatCells="Integer:B1,Long:B1,Short:B1,Double:C1,Float:C1,BigDecimal:C1,Date:D1")</t>
         </r>
       </text>
     </comment>
@@ -62,8 +62,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="171" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -130,14 +130,14 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -150,9 +150,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -190,7 +190,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -262,7 +262,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -436,29 +436,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.578125" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="5"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:4" ht="14.45" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="1"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>